<commit_message>
add guide company client status and generic PDF export
</commit_message>
<xml_diff>
--- a/web/flask/templates/guide_company_client_status.xlsx
+++ b/web/flask/templates/guide_company_client_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\inpdenaterm01\climberdb\git\web\flask\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E28B8E-1A90-4780-8258-4EE612212122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF1EA8F-6CB9-4036-AED3-F77D0AF1EDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C695E106-C865-4C24-8B38-EF7BD97409F5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Group Name</t>
   </si>
@@ -46,15 +46,6 @@
   </si>
   <si>
     <t>Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Special Use Permit Application</t>
-  </si>
-  <si>
-    <t>Climber's Fee</t>
-  </si>
-  <si>
-    <t>Entrance Fee</t>
   </si>
   <si>
     <t>Briefing Date</t>
@@ -66,7 +57,13 @@
     <t>Number of Climbers</t>
   </si>
   <si>
-    <t>Registration Complete</t>
+    <t>SUP Application Complete</t>
+  </si>
+  <si>
+    <t>Climbing Fee Paid</t>
+  </si>
+  <si>
+    <t>Entrance Fee Paid</t>
   </si>
 </sst>
 </file>
@@ -76,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,17 +101,9 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,12 +122,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF28100"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,26 +137,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,32 +528,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B44544-63B1-435B-9374-39A52C225470}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="2" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -584,21 +561,18 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:C1048576">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -629,7 +603,7 @@
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -637,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
show query link in exports
</commit_message>
<xml_diff>
--- a/web/flask/templates/guide_company_client_status.xlsx
+++ b/web/flask/templates/guide_company_client_status.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\inpdenaterm01\climberdb\git\web\flask\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\climberdb\git\web\flask\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF1EA8F-6CB9-4036-AED3-F77D0AF1EDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C695E106-C865-4C24-8B38-EF7BD97409F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Client Status" sheetId="1" r:id="rId1"/>
     <sheet name="Briefings" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Client Status'!$A:$F</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
@@ -157,8 +159,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="2" xr:uid="{2F999DE8-0384-429E-BDC0-10868407AAF1}"/>
-    <cellStyle name="Normal_Sheet1_1" xfId="1" xr:uid="{3DE9BF56-EB90-48BA-A8B5-FE88A26E8430}"/>
+    <cellStyle name="Normal_Sheet1" xfId="2"/>
+    <cellStyle name="Normal_Sheet1_1" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -527,12 +529,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B44544-63B1-435B-9374-39A52C225470}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +542,7 @@
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -590,7 +593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45155D04-140C-4C5C-986F-11A4A8D86BF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>